<commit_message>
feat: Add gender differentiation to metadata
</commit_message>
<xml_diff>
--- a/files/participant_metadata_reference.xlsx
+++ b/files/participant_metadata_reference.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timos\Desktop\VBT\bounce_analyser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timos\Desktop\BounceInsight\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1283B7BC-5569-4436-B884-1835AD6758A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A64E2B-32EF-48D9-BBC7-B4DCADF3E280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33560" yWindow="2540" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38490" yWindow="10440" windowWidth="19380" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="load_bounce" sheetId="8" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="11">
   <si>
     <t>participant</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>bodyweight_2</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9598DB-4ED8-4C8A-9310-A8F8A2906658}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -473,9 +482,10 @@
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="21.75" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -494,8 +504,11 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -514,8 +527,11 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -531,8 +547,11 @@
       <c r="E3">
         <v>67.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -548,8 +567,11 @@
       <c r="E4">
         <v>89.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -565,8 +587,11 @@
       <c r="E5">
         <v>79.900000000000006</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -582,8 +607,11 @@
       <c r="E6">
         <v>66.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>7</v>
       </c>
@@ -599,8 +627,11 @@
       <c r="E7">
         <v>85.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>8</v>
       </c>
@@ -616,8 +647,11 @@
       <c r="E8">
         <v>64.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>9</v>
       </c>
@@ -633,8 +667,11 @@
       <c r="E9">
         <v>82.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>10</v>
       </c>
@@ -650,8 +687,11 @@
       <c r="E10">
         <v>83.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>12</v>
       </c>
@@ -667,8 +707,11 @@
       <c r="E11">
         <v>92.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>13</v>
       </c>
@@ -684,8 +727,11 @@
       <c r="E12">
         <v>81.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>14</v>
       </c>
@@ -704,8 +750,11 @@
       <c r="F13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>15</v>
       </c>
@@ -721,8 +770,11 @@
       <c r="E14">
         <v>84.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>16</v>
       </c>
@@ -741,8 +793,11 @@
       <c r="F15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>17</v>
       </c>
@@ -758,8 +813,11 @@
       <c r="E16">
         <v>85.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>18</v>
       </c>
@@ -778,8 +836,11 @@
       <c r="F17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>19</v>
       </c>
@@ -795,8 +856,11 @@
       <c r="E18">
         <v>74.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>20</v>
       </c>
@@ -815,8 +879,11 @@
       <c r="F19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>21</v>
       </c>
@@ -832,8 +899,11 @@
       <c r="E20">
         <v>90.3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>22</v>
       </c>
@@ -849,8 +919,11 @@
       <c r="E21">
         <v>61.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>23</v>
       </c>
@@ -866,8 +939,11 @@
       <c r="E22">
         <v>97.4</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>24</v>
       </c>
@@ -883,8 +959,11 @@
       <c r="E23">
         <v>91.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>25</v>
       </c>
@@ -903,8 +982,11 @@
       <c r="F24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>26</v>
       </c>
@@ -920,8 +1002,11 @@
       <c r="E25">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>27</v>
       </c>
@@ -937,8 +1022,11 @@
       <c r="E26">
         <v>70.900000000000006</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>28</v>
       </c>
@@ -957,8 +1045,11 @@
       <c r="F27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>29</v>
       </c>
@@ -974,8 +1065,11 @@
       <c r="E28">
         <v>63.4</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>31</v>
       </c>
@@ -994,8 +1088,11 @@
       <c r="F29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>32</v>
       </c>
@@ -1011,8 +1108,11 @@
       <c r="E30">
         <v>59.1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>33</v>
       </c>
@@ -1028,8 +1128,11 @@
       <c r="E31">
         <v>89</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>34</v>
       </c>
@@ -1045,8 +1148,11 @@
       <c r="E32">
         <v>95.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>35</v>
       </c>
@@ -1062,8 +1168,11 @@
       <c r="E33">
         <v>63.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>36</v>
       </c>
@@ -1079,8 +1188,11 @@
       <c r="E34">
         <v>73.7</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>38</v>
       </c>
@@ -1096,8 +1208,11 @@
       <c r="E35">
         <v>71.7</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>39</v>
       </c>
@@ -1113,8 +1228,11 @@
       <c r="E36">
         <v>95.8</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>40</v>
       </c>
@@ -1129,6 +1247,9 @@
       </c>
       <c r="E37">
         <v>80.3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix, upt and feat: fix for ID12, paired ttest with averages and check_data
- fix: implemented a fix for Session 2 of participant 12, with manually setting baseline due to small offset shift in fp data during recording

- upt: added a more robust version of the ttest to work with averages in a subgroup of a bounce/nobounce group, more reliable test results and better data

- upt: Removed old methods regarding statistical analysis, to build again from ground up

- feat: Implemented Check_data command to visualize normality distributions and search for outliers which could cause the normality test to fail
</commit_message>
<xml_diff>
--- a/files/participant_metadata_reference.xlsx
+++ b/files/participant_metadata_reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timos\Desktop\BounceInsight\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A64E2B-32EF-48D9-BBC7-B4DCADF3E280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495810CD-33C5-4887-BBDC-258D21FC3C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="10440" windowWidth="19380" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="1330" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="load_bounce" sheetId="8" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>

</xml_diff>